<commit_message>
Update for fixing the remaining Facility and EI issues.
</commit_message>
<xml_diff>
--- a/PBR Issue AugSept2019/LDB permits not migrated.xlsx
+++ b/PBR Issue AugSept2019/LDB permits not migrated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\solid-waste-migration\PBR Issue AugSept2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D4AF15-3913-449D-8265-AECD0190B03E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F287C39D-06E4-444D-9023-A1BD5917DBE9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="447">
   <si>
     <t>MainPermitNumber</t>
   </si>
@@ -1327,31 +1327,40 @@
     <t>Fixes from Program</t>
   </si>
   <si>
-    <t>Should have EI added to 020-012D(SL) - they are different types - LEMIR RID 345631</t>
-  </si>
-  <si>
-    <t>Facility added, but EI… MFLID: 33786</t>
-  </si>
-  <si>
-    <t>Environmental interest not migrated - MFLID: 33784</t>
-  </si>
-  <si>
-    <t>associates to wrong Permit - 002-007D(L) needs EI for 002-008P(RM) added - MFLID: 32688</t>
-  </si>
-  <si>
-    <t>This type was NOT to be Migrated - search gets 011-026D(SL) - MFLID: 9220</t>
-  </si>
-  <si>
-    <t>This type was NOT to be Migrated - Facilty was inserted with no EI - MFLID: 33785</t>
-  </si>
-  <si>
-    <t>was added to facility 150028, but EI type was NOT to be migrated - MFLID: NONE</t>
-  </si>
-  <si>
-    <t>facility info added, needs added EI - MFLID:  14736</t>
-  </si>
-  <si>
-    <t>No Needs to be split from FAC-345938- like EIs - MFLID: 33864</t>
+    <t>028-040D(L), 028-030D(L) and 028-040(C&amp;D) are different phases of same site with same EI. Must make new Facility.</t>
+  </si>
+  <si>
+    <t>MFL_ID</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">associates to wrong Permit - 002-007D(L) needs EI for 002-008P(RM) added </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environmental interest not migrated </t>
+  </si>
+  <si>
+    <t>This type was NOT to be Migrated - search gets 011-026D(SL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This type was NOT to be Migrated - Facilty was inserted with no EI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should have EI added to 020-012D(SL) - they are different types - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">was added to facility 150028, but EI type was NOT to be migrated </t>
+  </si>
+  <si>
+    <t>Facility added, but EI missing. Must add EI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility info added, needs added EI </t>
+  </si>
+  <si>
+    <t>Facility added, needs EI added</t>
   </si>
 </sst>
 </file>
@@ -1436,7 +1445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1485,11 +1494,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1589,22 +1610,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BB7CC2A2-E065-4EF1-9281-09E7E1793B86}" name="Table1" displayName="Table1" ref="A1:S82" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:S82" xr:uid="{14D30FF3-018D-4D42-911C-0E416E48CDE4}"/>
-  <tableColumns count="19">
-    <tableColumn id="17" xr3:uid="{5CBA3AA5-0A18-47D3-845E-96B0F8D34050}" name="LEMIR RID" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BB7CC2A2-E065-4EF1-9281-09E7E1793B86}" name="Table1" displayName="Table1" ref="A1:T82" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:T82" xr:uid="{14D30FF3-018D-4D42-911C-0E416E48CDE4}"/>
+  <tableColumns count="20">
+    <tableColumn id="17" xr3:uid="{5CBA3AA5-0A18-47D3-845E-96B0F8D34050}" name="LEMIR RID" dataDxfId="6"/>
+    <tableColumn id="20" xr3:uid="{A73B4B84-E80E-45C1-A47C-A96E955A6D5E}" name="MFL_ID" dataDxfId="0"/>
     <tableColumn id="1" xr3:uid="{9998488B-7FD4-4EED-B03A-E5C96CA91462}" name="MainPermitNumber"/>
     <tableColumn id="2" xr3:uid="{8C8273C8-1EFD-4941-B3B4-99881F4DC70D}" name="FacilityName"/>
-    <tableColumn id="3" xr3:uid="{02C2F57A-5071-442F-B240-298DBB299408}" name="OperationStatus" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{0AF5C266-B12C-4D96-9D19-43236AE2D70B}" name="FacilityType" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{02C2F57A-5071-442F-B240-298DBB299408}" name="OperationStatus" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{0AF5C266-B12C-4D96-9D19-43236AE2D70B}" name="FacilityType" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{CE3B434D-E088-4B8A-9B59-8DA64799D827}" name="FacilityTypeDescription"/>
     <tableColumn id="6" xr3:uid="{82743D10-E043-49EB-A07E-BFBBC39487D6}" name="FacilityAddress"/>
     <tableColumn id="7" xr3:uid="{8754E4BE-89CE-4DB3-B134-7672A88BBB64}" name="City"/>
     <tableColumn id="8" xr3:uid="{41C80440-5553-4283-AFE9-8CD239FBF9F1}" name="State"/>
-    <tableColumn id="9" xr3:uid="{97C8CB1D-0B1B-46EB-A195-A6C6E0D83BFE}" name="ZipCode" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{97C8CB1D-0B1B-46EB-A195-A6C6E0D83BFE}" name="ZipCode" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{61205ADA-72E2-45FE-A9F2-A92C5193F360}" name="County"/>
-    <tableColumn id="11" xr3:uid="{0E4434AF-F30B-47F4-8BC3-E8D5A210B57E}" name="GWSystemInstalled" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{1792D564-3852-4C9F-B180-A27D8B9B4801}" name="MethaneSystemInstalled" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{0E4434AF-F30B-47F4-8BC3-E8D5A210B57E}" name="GWSystemInstalled" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{1792D564-3852-4C9F-B180-A27D8B9B4801}" name="MethaneSystemInstalled" dataDxfId="1"/>
     <tableColumn id="13" xr3:uid="{DE43B780-F1C4-49E2-8E1A-03214D33CBF4}" name="MailingAddress"/>
     <tableColumn id="14" xr3:uid="{0174FFF2-2FDE-4CD1-8850-29D81C243C10}" name="MailingCity"/>
     <tableColumn id="15" xr3:uid="{A5CF89FB-F208-426E-A765-3544E5A0AD23}" name="MailingState"/>
@@ -1901,195 +1923,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S82"/>
+  <dimension ref="A1:T82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5400" ySplit="11415" topLeftCell="O35" activePane="topRight"/>
-      <selection activeCell="A11" sqref="A11"/>
-      <selection pane="topRight" activeCell="R10" sqref="R10"/>
+      <pane xSplit="7770" ySplit="11415" topLeftCell="P35" activePane="topRight"/>
+      <selection activeCell="C12" sqref="C12"/>
+      <selection pane="topRight" activeCell="S26" sqref="S26"/>
       <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
       <selection pane="bottomRight" activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="68.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="68.7109375" customWidth="1"/>
-    <col min="7" max="7" width="64.85546875" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="22" style="2" customWidth="1"/>
-    <col min="13" max="13" width="27.28515625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="52" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" customWidth="1"/>
-    <col min="18" max="18" width="84.28515625" customWidth="1"/>
-    <col min="19" max="19" width="72.85546875" customWidth="1"/>
+    <col min="1" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="68.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="68.7109375" customWidth="1"/>
+    <col min="8" max="8" width="64.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="22" style="2" customWidth="1"/>
+    <col min="14" max="14" width="27.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="52" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="18.28515625" customWidth="1"/>
+    <col min="19" max="19" width="102.85546875" customWidth="1"/>
+    <col min="20" max="20" width="72.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>345578</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="15">
+        <v>32688</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>28</v>
       </c>
-      <c r="P2" t="s">
-        <v>23</v>
-      </c>
       <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
         <v>24</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>345584</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="13">
+        <v>33784</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O3" t="s">
@@ -2102,50 +2130,53 @@
         <v>26</v>
       </c>
       <c r="R3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="S3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>1983</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="14">
+        <v>9220</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>40</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>41</v>
       </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O4" t="s">
@@ -2158,50 +2189,53 @@
         <v>26</v>
       </c>
       <c r="R4" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="S4" s="18" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>345607</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="14">
+        <v>33785</v>
+      </c>
+      <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>33</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>47</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>41</v>
       </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O5" t="s">
@@ -2214,379 +2248,403 @@
         <v>26</v>
       </c>
       <c r="R5" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="S5" s="18" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>345631</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="13">
+        <v>33738</v>
+      </c>
+      <c r="C6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>53</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>54</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>55</v>
       </c>
-      <c r="I6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" t="s">
         <v>58</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>59</v>
       </c>
-      <c r="P6" t="s">
-        <v>23</v>
-      </c>
       <c r="Q6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R6" t="s">
         <v>56</v>
       </c>
-      <c r="R6" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S6" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>150028</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>62</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>63</v>
       </c>
-      <c r="I7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" t="s">
         <v>66</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>67</v>
       </c>
-      <c r="P7" t="s">
-        <v>23</v>
-      </c>
       <c r="Q7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R7" t="s">
         <v>64</v>
       </c>
-      <c r="R7" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S7" s="18" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>345658</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="13">
+        <v>33786</v>
+      </c>
+      <c r="C8" t="s">
         <v>68</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>71</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>72</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>63</v>
       </c>
-      <c r="I8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>65</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" t="s">
         <v>74</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>67</v>
       </c>
-      <c r="P8" t="s">
-        <v>23</v>
-      </c>
       <c r="Q8" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" t="s">
         <v>73</v>
       </c>
-      <c r="R8" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>8624</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="13">
+        <v>14736</v>
+      </c>
+      <c r="C9" t="s">
         <v>75</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>78</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>79</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>63</v>
       </c>
-      <c r="I9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>65</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O9" t="s">
         <v>81</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>67</v>
       </c>
-      <c r="P9" t="s">
-        <v>23</v>
-      </c>
       <c r="Q9" t="s">
+        <v>23</v>
+      </c>
+      <c r="R9" t="s">
         <v>80</v>
       </c>
-      <c r="R9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S9" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>345938</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="16" t="s">
+        <v>437</v>
+      </c>
+      <c r="C10" t="s">
         <v>82</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>86</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>87</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>88</v>
       </c>
-      <c r="I10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>90</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O10" t="s">
         <v>92</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>88</v>
       </c>
-      <c r="P10" t="s">
-        <v>23</v>
-      </c>
       <c r="Q10" t="s">
+        <v>23</v>
+      </c>
+      <c r="R10" t="s">
         <v>93</v>
       </c>
-      <c r="R10" s="17" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" t="s">
+      <c r="S10" s="17" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>345944</v>
+      </c>
+      <c r="B11" s="13">
+        <v>33870</v>
+      </c>
+      <c r="C11" t="s">
         <v>94</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>78</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>96</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>97</v>
       </c>
-      <c r="I11" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>99</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" t="s">
         <v>100</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>101</v>
       </c>
-      <c r="P11" t="s">
-        <v>23</v>
-      </c>
       <c r="Q11" t="s">
+        <v>23</v>
+      </c>
+      <c r="R11" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" t="s">
         <v>102</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>106</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>107</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>108</v>
       </c>
-      <c r="I12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>110</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O12" t="s">
@@ -2598,97 +2656,99 @@
       <c r="Q12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" t="s">
         <v>111</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>106</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>113</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>114</v>
       </c>
-      <c r="I13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>110</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O13" t="s">
         <v>113</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>114</v>
       </c>
-      <c r="P13" t="s">
-        <v>23</v>
-      </c>
       <c r="Q13" t="s">
+        <v>23</v>
+      </c>
+      <c r="R13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" t="s">
         <v>116</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>117</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>33</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>118</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>119</v>
       </c>
-      <c r="I14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>121</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O14" t="s">
@@ -2700,46 +2760,47 @@
       <c r="Q14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" t="s">
         <v>122</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>33</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>124</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>125</v>
       </c>
-      <c r="I15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>127</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O15" t="s">
@@ -2751,199 +2812,203 @@
       <c r="Q15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" t="s">
         <v>128</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>129</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>78</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>130</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>131</v>
       </c>
-      <c r="I16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>127</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O16" t="s">
         <v>133</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>134</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>135</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" t="s">
         <v>137</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>138</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>33</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>139</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>140</v>
       </c>
-      <c r="I17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>142</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O17" t="s">
         <v>143</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>144</v>
       </c>
-      <c r="P17" t="s">
-        <v>23</v>
-      </c>
       <c r="Q17" t="s">
+        <v>23</v>
+      </c>
+      <c r="R17" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" t="s">
         <v>146</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>147</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>33</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>148</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>149</v>
       </c>
-      <c r="I18" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>151</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O18" t="s">
         <v>152</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>153</v>
       </c>
-      <c r="P18" t="s">
-        <v>23</v>
-      </c>
       <c r="Q18" t="s">
+        <v>23</v>
+      </c>
+      <c r="R18" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" t="s">
         <v>155</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>156</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" t="s">
         <v>157</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>158</v>
       </c>
-      <c r="I19" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>160</v>
       </c>
-      <c r="L19" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O19" t="s">
@@ -2955,403 +3020,411 @@
       <c r="Q19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" t="s">
         <v>161</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>162</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>106</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>164</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>165</v>
       </c>
-      <c r="I20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="2" t="s">
+      <c r="J20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>167</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O20" t="s">
         <v>168</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>169</v>
       </c>
-      <c r="P20" t="s">
-        <v>23</v>
-      </c>
       <c r="Q20" t="s">
+        <v>23</v>
+      </c>
+      <c r="R20" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" t="s">
         <v>171</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>172</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>78</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>173</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>174</v>
       </c>
-      <c r="I21" t="s">
-        <v>23</v>
-      </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>176</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O21" t="s">
         <v>26</v>
       </c>
       <c r="P21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="Q21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="R21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" t="s">
         <v>177</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>178</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>20</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>179</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>180</v>
       </c>
-      <c r="I22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="2" t="s">
+      <c r="J22" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>182</v>
       </c>
-      <c r="L22" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O22" t="s">
         <v>183</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>169</v>
       </c>
-      <c r="P22" t="s">
-        <v>23</v>
-      </c>
       <c r="Q22" t="s">
+        <v>23</v>
+      </c>
+      <c r="R22" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" t="s">
         <v>185</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>186</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>106</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>187</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>188</v>
       </c>
-      <c r="I23" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="2" t="s">
+      <c r="J23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>190</v>
       </c>
-      <c r="L23" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O23" t="s">
         <v>191</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>192</v>
       </c>
-      <c r="P23" t="s">
-        <v>23</v>
-      </c>
       <c r="Q23" t="s">
+        <v>23</v>
+      </c>
+      <c r="R23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" t="s">
         <v>193</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>194</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>33</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>196</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>197</v>
       </c>
-      <c r="I24" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>199</v>
       </c>
-      <c r="L24" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O24" t="s">
         <v>200</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>125</v>
       </c>
-      <c r="P24" t="s">
-        <v>23</v>
-      </c>
       <c r="Q24" t="s">
+        <v>23</v>
+      </c>
+      <c r="R24" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" t="s">
         <v>201</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>202</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>106</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>203</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>204</v>
       </c>
-      <c r="I25" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>199</v>
       </c>
-      <c r="L25" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O25" t="s">
         <v>206</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>207</v>
       </c>
-      <c r="P25" t="s">
-        <v>23</v>
-      </c>
       <c r="Q25" t="s">
+        <v>23</v>
+      </c>
+      <c r="R25" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" t="s">
+      <c r="B26" s="2"/>
+      <c r="C26" t="s">
         <v>209</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>210</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>78</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>211</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>212</v>
       </c>
-      <c r="I26" t="s">
-        <v>23</v>
-      </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>214</v>
       </c>
-      <c r="L26" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N26" t="s">
+      <c r="N26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O26" t="s">
         <v>215</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>216</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>217</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" t="s">
         <v>219</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>220</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>33</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>222</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>223</v>
       </c>
-      <c r="I27" t="s">
-        <v>23</v>
-      </c>
-      <c r="J27" s="2" t="s">
+      <c r="J27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>225</v>
       </c>
-      <c r="L27" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O27" t="s">
@@ -3363,301 +3436,307 @@
       <c r="Q27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" t="s">
         <v>226</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>227</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>20</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>228</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>229</v>
       </c>
-      <c r="I28" t="s">
-        <v>23</v>
-      </c>
-      <c r="J28" s="2" t="s">
+      <c r="J28" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>231</v>
       </c>
-      <c r="L28" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N28" t="s">
+      <c r="N28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O28" t="s">
         <v>232</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>233</v>
       </c>
-      <c r="P28" t="s">
-        <v>23</v>
-      </c>
       <c r="Q28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R28" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" t="s">
         <v>234</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>235</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>237</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>238</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>239</v>
       </c>
-      <c r="I29" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" s="2" t="s">
+      <c r="J29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>241</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N29" t="s">
+      <c r="N29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O29" t="s">
         <v>242</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>243</v>
       </c>
-      <c r="P29" t="s">
-        <v>23</v>
-      </c>
       <c r="Q29" t="s">
+        <v>23</v>
+      </c>
+      <c r="R29" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" t="s">
+      <c r="B30" s="2"/>
+      <c r="C30" t="s">
         <v>244</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>245</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>86</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>238</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>239</v>
       </c>
-      <c r="I30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>241</v>
       </c>
-      <c r="L30" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N30" t="s">
+      <c r="N30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O30" t="s">
         <v>242</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>243</v>
       </c>
-      <c r="P30" t="s">
-        <v>23</v>
-      </c>
       <c r="Q30" t="s">
+        <v>23</v>
+      </c>
+      <c r="R30" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" t="s">
+      <c r="B31" s="2"/>
+      <c r="C31" t="s">
         <v>246</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>247</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>78</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>248</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>249</v>
       </c>
-      <c r="I31" t="s">
-        <v>23</v>
-      </c>
-      <c r="J31" s="2" t="s">
+      <c r="J31" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>251</v>
       </c>
-      <c r="L31" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N31" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O31" t="s">
         <v>26</v>
       </c>
       <c r="P31" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="Q31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="R31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" t="s">
         <v>252</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>253</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>255</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>256</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>257</v>
       </c>
-      <c r="I32" t="s">
-        <v>23</v>
-      </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>259</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>260</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="N32" t="s">
+      <c r="N32" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="O32" t="s">
         <v>261</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>262</v>
       </c>
-      <c r="P32" t="s">
-        <v>23</v>
-      </c>
       <c r="Q32" t="s">
+        <v>23</v>
+      </c>
+      <c r="R32" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" t="s">
         <v>263</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>264</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>33</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>265</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>266</v>
       </c>
-      <c r="I33" t="s">
-        <v>23</v>
-      </c>
-      <c r="J33" s="2" t="s">
+      <c r="J33" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>268</v>
       </c>
-      <c r="L33" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M33" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N33" t="s">
+      <c r="N33" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O33" t="s">
@@ -3669,1117 +3748,1169 @@
       <c r="Q33" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" t="s">
         <v>269</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>270</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>273</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>274</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>275</v>
       </c>
-      <c r="I34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>277</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N34" t="s">
+      <c r="N34" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O34" t="s">
         <v>278</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>279</v>
       </c>
-      <c r="P34" t="s">
-        <v>23</v>
-      </c>
       <c r="Q34" t="s">
+        <v>23</v>
+      </c>
+      <c r="R34" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" t="s">
+      <c r="B35" s="2"/>
+      <c r="C35" t="s">
         <v>281</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>282</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>86</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>284</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>275</v>
       </c>
-      <c r="I35" t="s">
-        <v>23</v>
-      </c>
-      <c r="J35" s="2" t="s">
+      <c r="J35" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>277</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N35" t="s">
+      <c r="N35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O35" t="s">
         <v>278</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
         <v>279</v>
       </c>
-      <c r="P35" t="s">
-        <v>23</v>
-      </c>
       <c r="Q35" t="s">
+        <v>23</v>
+      </c>
+      <c r="R35" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="B36" t="s">
+      <c r="B36" s="2"/>
+      <c r="C36" t="s">
         <v>285</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>286</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>287</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>288</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>289</v>
       </c>
-      <c r="I36" t="s">
-        <v>23</v>
-      </c>
-      <c r="J36" s="2" t="s">
+      <c r="J36" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>291</v>
       </c>
-      <c r="L36" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N36" t="s">
+      <c r="N36" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O36" t="s">
         <v>26</v>
       </c>
       <c r="P36" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="Q36" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="R36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" t="s">
+      <c r="B37" s="2"/>
+      <c r="C37" t="s">
         <v>292</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>293</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>106</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>295</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>296</v>
       </c>
-      <c r="I37" t="s">
-        <v>23</v>
-      </c>
-      <c r="J37" s="2" t="s">
+      <c r="J37" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>291</v>
       </c>
-      <c r="L37" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N37" t="s">
+      <c r="N37" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O37" t="s">
         <v>295</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>296</v>
       </c>
-      <c r="P37" t="s">
-        <v>23</v>
-      </c>
       <c r="Q37" t="s">
+        <v>23</v>
+      </c>
+      <c r="R37" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="B38" t="s">
+      <c r="B38" s="2"/>
+      <c r="C38" t="s">
         <v>298</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>299</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>273</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>300</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>301</v>
       </c>
-      <c r="I38" t="s">
-        <v>23</v>
-      </c>
-      <c r="J38" s="2" t="s">
+      <c r="J38" t="s">
+        <v>23</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>303</v>
       </c>
-      <c r="L38" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M38" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N38" t="s">
+      <c r="N38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O38" t="s">
         <v>304</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>305</v>
       </c>
-      <c r="P38" t="s">
-        <v>23</v>
-      </c>
       <c r="Q38" t="s">
+        <v>23</v>
+      </c>
+      <c r="R38" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="B39" t="s">
+      <c r="B39" s="2"/>
+      <c r="C39" t="s">
         <v>306</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>307</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>308</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>309</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>310</v>
       </c>
-      <c r="I39" t="s">
-        <v>23</v>
-      </c>
-      <c r="J39" s="2" t="s">
+      <c r="J39" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>312</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N39" t="s">
+      <c r="N39" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O39" t="s">
         <v>313</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>310</v>
       </c>
-      <c r="P39" t="s">
-        <v>23</v>
-      </c>
       <c r="Q39" t="s">
+        <v>23</v>
+      </c>
+      <c r="R39" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="B40" t="s">
+      <c r="B40" s="2"/>
+      <c r="C40" t="s">
         <v>314</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>315</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>287</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>316</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>317</v>
       </c>
-      <c r="I40" t="s">
-        <v>23</v>
-      </c>
-      <c r="J40" s="2" t="s">
+      <c r="J40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>312</v>
       </c>
-      <c r="L40" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M40" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N40" t="s">
+      <c r="N40" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O40" t="s">
         <v>319</v>
       </c>
-      <c r="O40" t="s">
+      <c r="P40" t="s">
         <v>320</v>
       </c>
-      <c r="P40" t="s">
-        <v>23</v>
-      </c>
       <c r="Q40" t="s">
+        <v>23</v>
+      </c>
+      <c r="R40" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="B41" t="s">
+      <c r="B41" s="2"/>
+      <c r="C41" t="s">
         <v>321</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>322</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>86</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>323</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>324</v>
       </c>
-      <c r="I41" t="s">
-        <v>23</v>
-      </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" t="s">
+        <v>23</v>
+      </c>
+      <c r="K41" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>326</v>
       </c>
-      <c r="L41" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M41" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N41" t="s">
+      <c r="N41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O41" t="s">
         <v>327</v>
       </c>
-      <c r="O41" t="s">
+      <c r="P41" t="s">
         <v>328</v>
       </c>
-      <c r="P41" t="s">
-        <v>23</v>
-      </c>
       <c r="Q41" t="s">
+        <v>23</v>
+      </c>
+      <c r="R41" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="B42" t="s">
+      <c r="B42" s="2"/>
+      <c r="C42" t="s">
         <v>330</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>331</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>273</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>332</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>324</v>
       </c>
-      <c r="I42" t="s">
-        <v>23</v>
-      </c>
-      <c r="J42" s="2" t="s">
+      <c r="J42" t="s">
+        <v>23</v>
+      </c>
+      <c r="K42" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>326</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N42" t="s">
+      <c r="N42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O42" t="s">
         <v>327</v>
       </c>
-      <c r="O42" t="s">
+      <c r="P42" t="s">
         <v>328</v>
       </c>
-      <c r="P42" t="s">
-        <v>23</v>
-      </c>
       <c r="Q42" t="s">
+        <v>23</v>
+      </c>
+      <c r="R42" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
-      <c r="B43" t="s">
+      <c r="B43" s="2"/>
+      <c r="C43" t="s">
         <v>333</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>334</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>273</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>336</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>337</v>
       </c>
-      <c r="I43" t="s">
-        <v>23</v>
-      </c>
-      <c r="J43" s="2" t="s">
+      <c r="J43" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>339</v>
       </c>
-      <c r="L43" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M43" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N43" t="s">
+      <c r="N43" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O43" t="s">
         <v>340</v>
       </c>
-      <c r="O43" t="s">
+      <c r="P43" t="s">
         <v>337</v>
       </c>
-      <c r="P43" t="s">
-        <v>23</v>
-      </c>
       <c r="Q43" t="s">
+        <v>23</v>
+      </c>
+      <c r="R43" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
-      <c r="B44" t="s">
+      <c r="B44" s="2"/>
+      <c r="C44" t="s">
         <v>341</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>342</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>273</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>343</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>344</v>
       </c>
-      <c r="I44" t="s">
-        <v>23</v>
-      </c>
-      <c r="J44" s="2" t="s">
+      <c r="J44" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>346</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N44" t="s">
+      <c r="N44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O44" t="s">
         <v>347</v>
       </c>
-      <c r="O44" t="s">
+      <c r="P44" t="s">
         <v>348</v>
       </c>
-      <c r="P44" t="s">
-        <v>23</v>
-      </c>
       <c r="Q44" t="s">
+        <v>23</v>
+      </c>
+      <c r="R44" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
-      <c r="B45" t="s">
+      <c r="B45" s="2"/>
+      <c r="C45" t="s">
         <v>349</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>350</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>106</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>351</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>352</v>
       </c>
-      <c r="I45" t="s">
-        <v>23</v>
-      </c>
-      <c r="J45" s="2" t="s">
+      <c r="J45" t="s">
+        <v>23</v>
+      </c>
+      <c r="K45" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
         <v>354</v>
       </c>
-      <c r="L45" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M45" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N45" t="s">
+      <c r="N45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O45" t="s">
         <v>355</v>
       </c>
-      <c r="O45" t="s">
+      <c r="P45" t="s">
         <v>356</v>
       </c>
-      <c r="P45" t="s">
-        <v>23</v>
-      </c>
       <c r="Q45" t="s">
+        <v>23</v>
+      </c>
+      <c r="R45" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
-      <c r="B46" t="s">
+      <c r="B46" s="2"/>
+      <c r="C46" t="s">
         <v>357</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>358</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>106</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>359</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
         <v>352</v>
       </c>
-      <c r="I46" t="s">
-        <v>23</v>
-      </c>
-      <c r="J46" s="2" t="s">
+      <c r="J46" t="s">
+        <v>23</v>
+      </c>
+      <c r="K46" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
         <v>354</v>
       </c>
-      <c r="L46" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M46" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N46" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O46" t="s">
         <v>355</v>
       </c>
-      <c r="O46" t="s">
+      <c r="P46" t="s">
         <v>356</v>
       </c>
-      <c r="P46" t="s">
-        <v>23</v>
-      </c>
       <c r="Q46" t="s">
+        <v>23</v>
+      </c>
+      <c r="R46" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="D48" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="G48" s="5" t="s">
+      <c r="H48" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="R48" s="5" t="s">
+      <c r="S48" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="S48" s="11"/>
-    </row>
-    <row r="49" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="T48" s="11"/>
+    </row>
+    <row r="49" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>6542</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2"/>
+      <c r="C49" t="s">
         <v>362</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="D49" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="G49" s="10" t="s">
+      <c r="H49" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="R49" s="2" t="s">
+      <c r="S49" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="S49" s="10" t="s">
+      <c r="T49" s="10" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>6542</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2"/>
+      <c r="C50" t="s">
         <v>306</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="G50" s="10" t="s">
+      <c r="H50" s="10" t="s">
         <v>420</v>
       </c>
-      <c r="R50" s="2" t="s">
+      <c r="S50" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="S50" s="10" t="s">
+      <c r="T50" s="10" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
-      <c r="G51" s="10"/>
-      <c r="S51" s="11"/>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B51" s="2"/>
+      <c r="H51" s="10"/>
+      <c r="T51" s="11"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>350995</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="6"/>
+      <c r="C52" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="G52" s="10"/>
-      <c r="R52" s="6" t="s">
+      <c r="H52" s="10"/>
+      <c r="S52" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="S52" s="11"/>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T52" s="11"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>345959</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="6"/>
+      <c r="C53" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="D53" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="G53" s="10" t="s">
+      <c r="H53" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="R53" s="6" t="s">
+      <c r="S53" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="S53" s="10" t="s">
+      <c r="T53" s="10" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>345958</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="6"/>
+      <c r="C54" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="D54" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="G54" s="10" t="s">
+      <c r="H54" s="10" t="s">
         <v>421</v>
       </c>
-      <c r="R54" s="6" t="s">
+      <c r="S54" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="S54" s="10" t="s">
+      <c r="T54" s="10" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
-      <c r="G55" s="10"/>
-      <c r="S55" s="11"/>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B55" s="2"/>
+      <c r="H55" s="10"/>
+      <c r="T55" s="11"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>10779</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2"/>
+      <c r="C56" t="s">
         <v>376</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>377</v>
       </c>
-      <c r="G56" s="10" t="s">
+      <c r="H56" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="R56" s="9" t="s">
+      <c r="S56" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="S56" s="6" t="s">
+      <c r="T56" s="6" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>346007</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2"/>
+      <c r="C57" t="s">
         <v>379</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>380</v>
       </c>
-      <c r="G57" s="10" t="s">
+      <c r="H57" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="R57" s="9" t="s">
+      <c r="S57" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="S57" s="6" t="s">
+      <c r="T57" s="6" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
-      <c r="G58" s="10"/>
-      <c r="R58" s="9"/>
-      <c r="S58" s="11"/>
-    </row>
-    <row r="59" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="B58" s="2"/>
+      <c r="H58" s="10"/>
+      <c r="S58" s="9"/>
+      <c r="T58" s="11"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>11910</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="2"/>
+      <c r="C59" t="s">
         <v>382</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>383</v>
       </c>
-      <c r="G59" s="10" t="s">
+      <c r="H59" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="R59" s="7" t="s">
+      <c r="S59" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="S59" s="11" t="s">
+      <c r="T59" s="11" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
-      <c r="R60" s="9"/>
-      <c r="S60" s="11"/>
-    </row>
-    <row r="61" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="B60" s="2"/>
+      <c r="S60" s="9"/>
+      <c r="T60" s="11"/>
+    </row>
+    <row r="61" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>350997</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="2"/>
+      <c r="C61" t="s">
         <v>385</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>386</v>
       </c>
-      <c r="G61" s="10" t="s">
+      <c r="H61" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="R61" s="7" t="s">
+      <c r="S61" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="S61" s="6" t="s">
+      <c r="T61" s="6" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
-      <c r="R62" s="9"/>
-      <c r="S62" s="11"/>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B62" s="2"/>
+      <c r="S62" s="9"/>
+      <c r="T62" s="11"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>345994</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="2"/>
+      <c r="C63" t="s">
         <v>388</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>389</v>
       </c>
-      <c r="G63" s="10" t="s">
+      <c r="H63" s="10" t="s">
         <v>426</v>
       </c>
-      <c r="R63" s="7" t="s">
+      <c r="S63" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="S63" s="6" t="s">
+      <c r="T63" s="6" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
-      <c r="G64" s="10"/>
-      <c r="R64" s="9"/>
-      <c r="S64" s="11"/>
-    </row>
-    <row r="65" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="B64" s="2"/>
+      <c r="H64" s="10"/>
+      <c r="S64" s="9"/>
+      <c r="T64" s="11"/>
+    </row>
+    <row r="65" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>350990</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="2"/>
+      <c r="C65" t="s">
         <v>391</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>392</v>
       </c>
-      <c r="G65" s="10" t="s">
+      <c r="H65" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="R65" s="7" t="s">
+      <c r="S65" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="S65" s="6" t="s">
+      <c r="T65" s="6" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
-      <c r="G66" s="10"/>
-      <c r="R66" s="9"/>
-      <c r="S66" s="11"/>
-    </row>
-    <row r="67" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="B66" s="2"/>
+      <c r="H66" s="10"/>
+      <c r="S66" s="9"/>
+      <c r="T66" s="11"/>
+    </row>
+    <row r="67" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>351000</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="2"/>
+      <c r="C67" t="s">
         <v>394</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>395</v>
       </c>
-      <c r="G67" s="10" t="s">
+      <c r="H67" s="10" t="s">
         <v>428</v>
       </c>
-      <c r="R67" s="7" t="s">
+      <c r="S67" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="S67" s="6" t="s">
+      <c r="T67" s="6" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
-      <c r="G68" s="10"/>
-      <c r="R68" s="9"/>
-      <c r="S68" s="11"/>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B68" s="2"/>
+      <c r="H68" s="10"/>
+      <c r="S68" s="9"/>
+      <c r="T68" s="11"/>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>155874</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="2"/>
+      <c r="C69" t="s">
         <v>397</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>398</v>
       </c>
-      <c r="G69" s="10" t="s">
+      <c r="H69" s="10" t="s">
         <v>429</v>
       </c>
-      <c r="R69" s="9" t="s">
+      <c r="S69" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="S69" s="6" t="s">
+      <c r="T69" s="6" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
-      <c r="G70" s="10"/>
-      <c r="R70" s="9"/>
-      <c r="S70" s="11"/>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B70" s="2"/>
+      <c r="H70" s="10"/>
+      <c r="S70" s="9"/>
+      <c r="T70" s="11"/>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>350987</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="2"/>
+      <c r="C71" t="s">
         <v>400</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>401</v>
       </c>
-      <c r="G71" s="10" t="s">
+      <c r="H71" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="R71" s="9" t="s">
+      <c r="S71" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="S71" s="6" t="s">
+      <c r="T71" s="6" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
-      <c r="G72" s="10"/>
-      <c r="R72" s="9"/>
-      <c r="S72" s="11"/>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B72" s="2"/>
+      <c r="H72" s="10"/>
+      <c r="S72" s="9"/>
+      <c r="T72" s="11"/>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>350989</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="2"/>
+      <c r="C73" t="s">
         <v>403</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>404</v>
       </c>
-      <c r="G73" s="10" t="s">
+      <c r="H73" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="R73" s="9" t="s">
+      <c r="S73" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="S73" s="6" t="s">
+      <c r="T73" s="6" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
-      <c r="R74" s="9"/>
-      <c r="S74" s="11"/>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+      <c r="S74" s="9"/>
+      <c r="T74" s="11"/>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>350991</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="2"/>
+      <c r="C75" t="s">
         <v>406</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>407</v>
       </c>
-      <c r="G75" s="10" t="s">
+      <c r="H75" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="R75" s="7" t="s">
+      <c r="S75" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="S75" s="6" t="s">
+      <c r="T75" s="6" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
-      <c r="R76" s="9"/>
-      <c r="S76" s="11"/>
-    </row>
-    <row r="77" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="B76" s="2"/>
+      <c r="S76" s="9"/>
+      <c r="T76" s="11"/>
+    </row>
+    <row r="77" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>149872</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="2"/>
+      <c r="C77" t="s">
         <v>409</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>410</v>
       </c>
-      <c r="G77" s="10" t="s">
+      <c r="H77" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="R77" s="7" t="s">
+      <c r="S77" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="S77" s="11"/>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T77" s="11"/>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
-      <c r="R78" s="9"/>
-      <c r="S78" s="11"/>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B78" s="2"/>
+      <c r="S78" s="9"/>
+      <c r="T78" s="11"/>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
-      <c r="B79" t="s">
+      <c r="B79" s="2"/>
+      <c r="C79" t="s">
         <v>412</v>
       </c>
-      <c r="R79" s="7" t="s">
+      <c r="S79" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="S79" s="11"/>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T79" s="11"/>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
-      <c r="S80" s="11"/>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B80" s="2"/>
+      <c r="T80" s="11"/>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
-      <c r="S81" s="11"/>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B81" s="2"/>
+      <c r="T81" s="11"/>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
-      <c r="S82" s="11"/>
+      <c r="B82" s="2"/>
+      <c r="T82" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>